<commit_message>
Fixed bug in dummy data for injecting user with wrong username
</commit_message>
<xml_diff>
--- a/DummyData/V2 - DummyData.xlsx
+++ b/DummyData/V2 - DummyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repository\SocialServ\DummyData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38E1718-5C88-41B6-A57F-ABAC66C059A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6F1566-E7B6-4AE5-89C6-B43D1B641135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{AC1699A3-039E-419B-BD7C-83C7FE3FD7D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{AC1699A3-039E-419B-BD7C-83C7FE3FD7D3}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="posts" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,9 +55,6 @@
     <t>platform_admin</t>
   </si>
   <si>
-    <t>sse_user</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -143,12 +139,6 @@
     <t>guest</t>
   </si>
   <si>
-    <t>platform_admin, sse_user</t>
-  </si>
-  <si>
-    <t>soserve_admin, sse_user</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -170,9 +160,6 @@
     <t>Project 2022</t>
   </si>
   <si>
-    <t>platform_admin, soserve_admin, sse_user</t>
-  </si>
-  <si>
     <t>space_pic</t>
   </si>
   <si>
@@ -309,6 +296,18 @@
   </si>
   <si>
     <t>Project2022.jpg</t>
+  </si>
+  <si>
+    <t>platform_user</t>
+  </si>
+  <si>
+    <t>soserve_admin, platform_user</t>
+  </si>
+  <si>
+    <t>platform_admin, platform_user</t>
+  </si>
+  <si>
+    <t>platform_admin, soserve_admin, platform_user</t>
   </si>
 </sst>
 </file>
@@ -664,7 +663,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +681,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -690,15 +689,15 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +710,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,15 +736,15 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +757,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,40 +767,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
       <c r="L1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -809,37 +808,37 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
       <c r="D2" s="1">
         <v>31992</v>
       </c>
       <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
       <c r="L2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -847,75 +846,75 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>35462</v>
       </c>
       <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
         <v>37289</v>
       </c>
       <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
       <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
       <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
         <v>23</v>
       </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
       <c r="L4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -938,31 +937,31 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -975,17 +974,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -993,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1001,12 +1000,12 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1021,55 +1020,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D258298A-1E98-479F-9664-A76E902BF515}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1081,13 +1080,13 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1110,223 +1109,223 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1338,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25BBF9C-5205-40BF-88D6-6EAEB07A9F50}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,43 +1348,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>62</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1396,10 +1395,10 @@
         <v>44764</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1410,10 +1409,10 @@
         <v>44770</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1424,27 +1423,27 @@
         <v>44765</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1">
         <v>44766</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s">
         <v>2</v>
@@ -1452,16 +1451,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1">
         <v>44768</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1472,10 +1471,10 @@
         <v>44769</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1486,13 +1485,13 @@
         <v>44771</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K8" t="s">
         <v>2</v>
@@ -1501,7 +1500,7 @@
         <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1512,13 +1511,13 @@
         <v>44767</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1529,13 +1528,13 @@
         <v>44772</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1546,19 +1545,19 @@
         <v>44773</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1569,30 +1568,30 @@
         <v>44774</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1">
         <v>44775</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>